<commit_message>
Update Actividad 1.3 (Desarrollo).xlsx
</commit_message>
<xml_diff>
--- a/Actividad 1.3/Actividad 1.3 (Desarrollo).xlsx
+++ b/Actividad 1.3/Actividad 1.3 (Desarrollo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorio Github\Lab-III---LucasBaez\Actividad 1.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEBACBF-3D4E-46D5-92FA-0B57332A65BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F4DC67-8396-475B-9B6C-C74FD823B66B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C44F5A90-A0FE-4995-94F5-F8D8187F7333}"/>
+    <workbookView xWindow="20370" yWindow="-1635" windowWidth="29040" windowHeight="15840" xr2:uid="{C44F5A90-A0FE-4995-94F5-F8D8187F7333}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Fecha Inicio</t>
   </si>
   <si>
-    <t>date , not null</t>
-  </si>
-  <si>
     <t>Fecha Final</t>
   </si>
   <si>
@@ -215,6 +212,15 @@
   </si>
   <si>
     <t>Actividad 1.3</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>varchar[100],not null</t>
+  </si>
+  <si>
+    <t>date , not null , check (&lt;= getdate())</t>
   </si>
 </sst>
 </file>
@@ -401,40 +407,47 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -445,13 +458,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -478,15 +484,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
+      <xdr:colOff>695326</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>428626</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -500,9 +506,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4505325" y="1914525"/>
-          <a:ext cx="2019301" cy="19050"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4505326" y="1933575"/>
+          <a:ext cx="1866899" cy="161925"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -890,243 +896,235 @@
   <dimension ref="B1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:N17"/>
+      <selection activeCell="B1" sqref="B1:N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="19"/>
+      <c r="G2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="14" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="15"/>
-      <c r="I4" s="17" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="18"/>
+      <c r="I4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="11" t="s">
+      <c r="J4" s="14"/>
+      <c r="K4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="12"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="8"/>
-      <c r="I5" s="7" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="4"/>
+      <c r="I5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="7" t="s">
+      <c r="J5" s="4"/>
+      <c r="K5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="4"/>
     </row>
     <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="8"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="2" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="4"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2" t="s">
+      <c r="J6" s="12"/>
+      <c r="K6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="11"/>
+      <c r="M6" s="12"/>
+    </row>
+    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="K7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I7" s="7" t="s">
+      <c r="L7" s="11"/>
+      <c r="M7" s="12"/>
+    </row>
+    <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="7" t="s">
+      <c r="J8" s="4"/>
+      <c r="K8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="18"/>
-    </row>
-    <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I8" s="7" t="s">
+      <c r="L8" s="8"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="14"/>
+      <c r="I9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="7" t="s">
+      <c r="J9" s="4"/>
+      <c r="K9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="4"/>
+      <c r="I10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="12"/>
-      <c r="I9" s="7" t="s">
+      <c r="J10" s="4"/>
+      <c r="K10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="2" t="s">
+      <c r="L10" s="11"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="I11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="8"/>
-      <c r="I10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="7" t="s">
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="4"/>
+      <c r="I12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="8"/>
-    </row>
-    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="3"/>
-      <c r="I11" s="7" t="s">
+      <c r="J12" s="4"/>
+      <c r="K12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L11" s="5"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="8"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="7" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="7" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:M11"/>
+  <mergeCells count="41">
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D12:G12"/>
@@ -1143,8 +1141,27 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>